<commit_message>
Corrected mishaps in agro dealers and ensured performance indicator values are displayed on charts as expected
</commit_message>
<xml_diff>
--- a/src/main/webapp/documents/population/download_files/SN PUF.xlsx
+++ b/src/main/webapp/documents/population/download_files/SN PUF.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Farmers" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Bank account number</t>
   </si>
   <si>
-    <t xml:space="preserve">SOL ID</t>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
     <t xml:space="preserve">Equity branch name</t>
@@ -517,19 +517,19 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1376518218624"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.9959514170041"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,11 +632,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1376518218624"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,8 +710,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.99595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>